<commit_message>
fix bug upload file
</commit_message>
<xml_diff>
--- a/assets/soal/soal.xlsx
+++ b/assets/soal/soal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -60,6 +60,72 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Ibukota Indonesia</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Lampung</t>
+  </si>
+  <si>
+    <t>Medan</t>
+  </si>
+  <si>
+    <t>Indonesia Bagian dari Benua</t>
+  </si>
+  <si>
+    <t>Eropa</t>
+  </si>
+  <si>
+    <t>Antartika</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Afrika</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>1 Jam sama dengan</t>
+  </si>
+  <si>
+    <t>2 menit</t>
+  </si>
+  <si>
+    <t>50 detik</t>
+  </si>
+  <si>
+    <t>40 detik</t>
+  </si>
+  <si>
+    <t>Pilihan_D</t>
+  </si>
+  <si>
+    <t>60 menit</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Hokage Konoha ke 1</t>
+  </si>
+  <si>
+    <t>Hashirama</t>
+  </si>
+  <si>
+    <t>Kakashi</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -393,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -451,25 +517,25 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -477,184 +543,69 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>11</v>
+      <c r="G6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>